<commit_message>
Initial POC voltage setable
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energinet.local\endk_funktion\Projekter\EffektGruppen\13_Medarbejdermapper\CVL\PP-MTB\Powerfactory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\energinet.local\endk_funktion\Projekter\EffektGruppen\13_Medarbejdermapper\CVL\PP-MTB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="PSCAD Compliers" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$1:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input!$A$1:$N$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="136">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>Fredericia</t>
+  </si>
+  <si>
+    <t>droop (%)</t>
   </si>
 </sst>
 </file>
@@ -1110,28 +1113,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" style="11" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10" style="11" customWidth="1"/>
     <col min="5" max="5" width="8" style="11" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="11"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" customWidth="1"/>
-    <col min="11" max="11" width="42.5703125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" customWidth="1"/>
+    <col min="12" max="12" width="42.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>60</v>
       </c>
@@ -1150,32 +1156,35 @@
       <c r="F1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="30">
         <v>10</v>
       </c>
@@ -1191,67 +1200,70 @@
       <c r="F2" s="30">
         <v>15</v>
       </c>
-      <c r="G2" s="29">
-        <v>0</v>
+      <c r="G2" s="30">
+        <v>2</v>
       </c>
       <c r="H2" s="29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="29">
+        <v>1</v>
+      </c>
+      <c r="J2" s="29">
         <v>2</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="29">
+      <c r="M2" s="29">
         <v>2</v>
       </c>
-      <c r="M2" s="29">
+      <c r="N2" s="29">
         <v>32</v>
       </c>
-      <c r="N2" s="29">
+      <c r="O2" s="29">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="26" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H4" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="L4" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="O4" s="26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="31" t="s">
+    <row r="5" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="31"/>
       <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="26" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H6" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="26" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H7" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="26" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H8" s="26" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1433,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G2" s="19">
@@ -1550,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G3" s="19">
@@ -1667,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G4" s="19">
@@ -1784,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G5" s="19">
@@ -1901,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G6" s="19">
@@ -2018,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G7" s="19">
@@ -2135,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G8" s="19">
@@ -2252,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G9" s="19">
@@ -2369,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G10" s="19">
@@ -2486,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G11" s="19">
@@ -2603,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G12" s="19">
@@ -2720,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G13" s="19">
@@ -2837,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G14" s="19">
@@ -2954,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G15" s="19">
@@ -3071,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G16" s="19">
@@ -3188,7 +3200,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G17" s="19">
@@ -3305,7 +3317,7 @@
         <v>0.7</v>
       </c>
       <c r="F18" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G18" s="19">
@@ -3422,7 +3434,7 @@
         <v>0.7</v>
       </c>
       <c r="F19" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G19" s="19">
@@ -3539,7 +3551,7 @@
         <v>0.7</v>
       </c>
       <c r="F20" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G20" s="19">
@@ -3656,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G21" s="19">
@@ -3773,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G22" s="19">
@@ -3890,7 +3902,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="23">
-        <f>Input!H2</f>
+        <f>Input!I2</f>
         <v>1</v>
       </c>
       <c r="G23" s="19">
@@ -4014,7 +4026,7 @@
         <v>0.7</v>
       </c>
       <c r="F24" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G24" s="19">
@@ -4131,7 +4143,7 @@
         <v>0.5</v>
       </c>
       <c r="F25" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G25" s="19">
@@ -4249,7 +4261,7 @@
         <v>0.7</v>
       </c>
       <c r="F26" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G26" s="19">
@@ -4366,7 +4378,7 @@
         <v>0.7</v>
       </c>
       <c r="F27" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G27" s="19">
@@ -4483,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G28" s="19">
@@ -4600,7 +4612,7 @@
         <v>0.7</v>
       </c>
       <c r="F29" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G29" s="19">
@@ -4717,7 +4729,7 @@
         <v>0.3</v>
       </c>
       <c r="F30" s="23">
-        <f>Input!I2</f>
+        <f>Input!J2</f>
         <v>2</v>
       </c>
       <c r="G30" s="19">
@@ -4834,7 +4846,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G31" s="19">
@@ -4951,7 +4963,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G32" s="19">
@@ -5068,7 +5080,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="20">
-        <f>Input!G2</f>
+        <f>Input!H2</f>
         <v>0</v>
       </c>
       <c r="G33" s="19">
@@ -5185,7 +5197,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="23">
-        <f>Input!I2</f>
+        <f>Input!J2</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">

</xml_diff>

<commit_message>
Protection SCR and sim stop updated
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="308" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" tabRatio="308"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="8" r:id="rId1"/>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,9 +2915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10117,7 +10117,7 @@
         <v>126.60000000000001</v>
       </c>
       <c r="K80" s="38" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
@@ -10245,7 +10245,7 @@
         <v>122</v>
       </c>
       <c r="K81" s="38" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
@@ -10349,7 +10349,7 @@
         <v>5.8</v>
       </c>
       <c r="K82" s="38" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L82" s="38"/>
       <c r="M82" s="38"/>
@@ -10470,7 +10470,7 @@
         <v>5.32</v>
       </c>
       <c r="K83" s="38" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>

</xml_diff>

<commit_message>
Force FSM added + RMS included updated (Testcases)
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" tabRatio="308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" tabRatio="308" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="8" r:id="rId1"/>
@@ -943,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1076,6 +1076,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1384,7 +1387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1511,9 +1514,9 @@
       <c r="C10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
@@ -1863,16 +1866,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
@@ -2915,7 +2918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -2988,78 +2991,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="49" t="s">
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="52" t="s">
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="49" t="s">
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="52" t="s">
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="49" t="s">
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="52" t="s">
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="49" t="s">
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="54"/>
+      <c r="AR1" s="55"/>
+      <c r="AS1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="AT1" s="50"/>
-      <c r="AU1" s="50"/>
-      <c r="AV1" s="51"/>
-      <c r="AW1" s="52" t="s">
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="AX1" s="53"/>
-      <c r="AY1" s="53"/>
-      <c r="AZ1" s="54"/>
-      <c r="BA1" s="49" t="s">
+      <c r="AX1" s="54"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="55"/>
+      <c r="BA1" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="BB1" s="50"/>
-      <c r="BC1" s="50"/>
-      <c r="BD1" s="51"/>
-      <c r="BE1" s="52" t="s">
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="BF1" s="53"/>
-      <c r="BG1" s="53"/>
-      <c r="BH1" s="54"/>
-      <c r="BI1" s="49" t="s">
+      <c r="BF1" s="54"/>
+      <c r="BG1" s="54"/>
+      <c r="BH1" s="55"/>
+      <c r="BI1" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="BJ1" s="50"/>
-      <c r="BK1" s="50"/>
-      <c r="BL1" s="51"/>
+      <c r="BJ1" s="51"/>
+      <c r="BK1" s="51"/>
+      <c r="BL1" s="52"/>
     </row>
     <row r="2" spans="1:64" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -3259,9 +3262,9 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B3" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C3" s="15" t="b">
         <f>TRUE</f>
@@ -3332,9 +3335,9 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B4" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C4" s="15" t="b">
         <f>TRUE</f>
@@ -3405,9 +3408,9 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B5" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C5" s="15" t="b">
         <f>TRUE</f>
@@ -3478,9 +3481,9 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B6" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C6" s="15" t="b">
         <f>TRUE</f>
@@ -3551,9 +3554,9 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B7" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C7" s="15" t="b">
         <f>TRUE</f>
@@ -3624,9 +3627,9 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B8" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C8" s="15" t="b">
         <f>TRUE</f>
@@ -3697,9 +3700,9 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B9" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C9" s="15" t="b">
         <f>TRUE</f>
@@ -3770,9 +3773,9 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B10" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C10" s="15" t="b">
         <f>TRUE</f>
@@ -3843,9 +3846,9 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B11" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C11" s="41" t="b">
         <f>FALSE</f>
@@ -3931,9 +3934,9 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B12" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C12" s="15" t="b">
         <f>TRUE</f>
@@ -4019,9 +4022,9 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B13" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C13" s="41" t="b">
         <f>FALSE</f>
@@ -4107,9 +4110,9 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B14" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C14" s="41" t="b">
         <f>FALSE</f>
@@ -4195,9 +4198,9 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B15" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C15" s="41" t="b">
         <f>FALSE</f>
@@ -4283,9 +4286,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B16" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C16" s="41" t="b">
         <f>FALSE</f>
@@ -4371,9 +4374,9 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B17" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C17" s="15" t="b">
         <f>TRUE</f>
@@ -4482,9 +4485,9 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B18" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C18" s="15" t="b">
         <f>TRUE</f>
@@ -4572,9 +4575,9 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B19" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C19" s="15" t="b">
         <f>TRUE</f>
@@ -4662,9 +4665,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B20" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C20" s="15" t="b">
         <f>TRUE</f>
@@ -4761,9 +4764,9 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B21" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C21" s="15" t="b">
         <f>TRUE</f>
@@ -4872,7 +4875,8 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="41" t="b">
+      <c r="B22" s="47" t="b">
+        <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="C22" s="15" t="b">
@@ -4966,9 +4970,9 @@
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B23" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C23" s="15" t="b">
         <f>TRUE</f>
@@ -5055,9 +5059,9 @@
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B24" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C24" s="15" t="b">
         <f>TRUE</f>
@@ -5146,9 +5150,9 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B25" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C25" s="15" t="b">
         <f>TRUE</f>
@@ -5237,9 +5241,9 @@
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B26" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C26" s="15" t="b">
         <f>TRUE</f>
@@ -5328,9 +5332,9 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B27" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C27" s="15" t="b">
         <f>TRUE</f>
@@ -5419,9 +5423,9 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B28" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C28" s="15" t="b">
         <f>TRUE</f>
@@ -5510,9 +5514,9 @@
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B29" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C29" s="15" t="b">
         <f>TRUE</f>
@@ -5601,9 +5605,9 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B30" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C30" s="41" t="b">
         <v>1</v>
@@ -5687,9 +5691,9 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B31" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C31" s="41" t="b">
         <f>$S31&gt;$E31</f>
@@ -5775,9 +5779,9 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B32" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C32" s="41" t="b">
         <f>$S32&gt;$E32</f>
@@ -5863,9 +5867,9 @@
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B33" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C33" s="41" t="b">
         <v>1</v>
@@ -5949,9 +5953,9 @@
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B34" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C34" s="41" t="b">
         <f>$S34&lt;$E34</f>
@@ -6037,9 +6041,9 @@
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B35" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C35" s="41" t="b">
         <f>$S35&lt;$E35</f>
@@ -6125,9 +6129,9 @@
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B36" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C36" s="41" t="b">
         <v>1</v>
@@ -6211,9 +6215,9 @@
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B37" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C37" s="41" t="b">
         <f>$S37&gt;$E37</f>
@@ -6299,9 +6303,9 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B38" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C38" s="41" t="b">
         <f>$S38&gt;$E38</f>
@@ -6387,9 +6391,9 @@
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B39" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C39" s="41" t="b">
         <v>1</v>
@@ -6473,9 +6477,9 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B40" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C40" s="41" t="b">
         <f>$S40&lt;$E40</f>
@@ -6561,9 +6565,9 @@
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B41" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C41" s="41" t="b">
         <f>$S41&lt;$E41</f>
@@ -6649,9 +6653,9 @@
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B42" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C42" s="41" t="b">
         <v>0</v>
@@ -6734,9 +6738,9 @@
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B43" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C43" s="41" t="b">
         <v>0</v>
@@ -6819,9 +6823,9 @@
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B44" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C44" s="41" t="b">
         <v>1</v>
@@ -6908,9 +6912,9 @@
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B45" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C45" s="41" t="b">
         <v>1</v>
@@ -6997,9 +7001,9 @@
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B46" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C46" s="41" t="b">
         <v>1</v>
@@ -7082,9 +7086,9 @@
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B47" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C47" s="41" t="b">
         <v>1</v>
@@ -7167,9 +7171,9 @@
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B48" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C48" s="41" t="b">
         <v>1</v>
@@ -7277,9 +7281,9 @@
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B49" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C49" s="41" t="b">
         <v>1</v>
@@ -7387,9 +7391,9 @@
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B50" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C50" s="41" t="b">
         <v>1</v>
@@ -7497,9 +7501,9 @@
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B51" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C51" s="41" t="b">
         <v>1</v>
@@ -7608,9 +7612,9 @@
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B52" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C52" s="41" t="b">
         <v>1</v>
@@ -8318,9 +8322,9 @@
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B61" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C61" s="41" t="b">
         <v>1</v>
@@ -8410,9 +8414,9 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B62" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C62" s="41" t="b">
         <v>1</v>
@@ -8499,9 +8503,9 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B63" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C63" s="41" t="b">
         <v>1</v>
@@ -8600,9 +8604,9 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B64" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C64" s="41" t="b">
         <v>1</v>
@@ -8701,9 +8705,9 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B65" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C65" s="41" t="b">
         <v>1</v>
@@ -8802,9 +8806,9 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B66" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C66" s="41" t="b">
         <v>1</v>
@@ -8890,9 +8894,9 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B67" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C67" s="41" t="b">
         <v>1</v>
@@ -8979,9 +8983,9 @@
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B68" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C68" s="41" t="b">
         <v>1</v>
@@ -9068,9 +9072,9 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B69" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C69" s="41" t="b">
         <v>1</v>
@@ -9157,9 +9161,9 @@
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B70" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C70" s="41" t="b">
         <v>1</v>
@@ -9246,9 +9250,9 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B71" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C71" s="41" t="b">
         <v>1</v>
@@ -9334,9 +9338,9 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B72" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C72" s="41" t="b">
         <v>1</v>
@@ -9423,9 +9427,9 @@
       <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B73" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C73" s="41" t="b">
         <v>1</v>
@@ -9512,9 +9516,9 @@
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B74" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C74" s="41" t="b">
         <v>1</v>
@@ -9601,9 +9605,9 @@
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B75" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C75" s="41" t="b">
         <v>1</v>
@@ -9690,9 +9694,9 @@
       <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B76" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C76" s="41" t="b">
         <v>1</v>
@@ -9797,9 +9801,9 @@
       <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B77" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C77" s="41" t="b">
         <v>1</v>
@@ -9891,9 +9895,9 @@
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B78" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C78" s="41" t="b">
         <v>1</v>
@@ -9988,9 +9992,9 @@
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B79" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C79" s="41" t="b">
         <v>1</v>
@@ -10086,9 +10090,9 @@
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B80" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C80" s="41" t="b">
         <v>1</v>
@@ -10214,9 +10218,9 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B81" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C81" s="41" t="b">
         <v>1</v>
@@ -10318,9 +10322,9 @@
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B82" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C82" s="41" t="b">
         <v>1</v>
@@ -10439,9 +10443,9 @@
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="41" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="B83" s="47" t="b">
+        <f>TRUE</f>
+        <v>1</v>
       </c>
       <c r="C83" s="41" t="b">
         <v>1</v>

</xml_diff>